<commit_message>
configured chp verify cholera case task
</commit_message>
<xml_diff>
--- a/forms/app/cha_verify_case.xlsx
+++ b/forms/app/cha_verify_case.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -742,10 +742,10 @@
   </sheetPr>
   <dimension ref="A1:AJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+      <selection pane="bottomLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3561,7 +3561,7 @@
   </sheetPr>
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -3623,7 +3623,7 @@
       </c>
       <c r="C2" s="32" t="n">
         <f aca="true">NOW()</f>
-        <v>45266.4298380143</v>
+        <v>45266.45131422</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>94</v>

</xml_diff>